<commit_message>
Get all annual expense report
</commit_message>
<xml_diff>
--- a/FinancialPlanningBE/FinancialPlanning.Service/Template/Annual Expense Report.xlsx
+++ b/FinancialPlanningBE/FinancialPlanning.Service/Template/Annual Expense Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\FinancialPlanning\financial-planning\FinancialPlanningBE\FinancialPlanning.Service\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,7 +47,7 @@
     <t>Biggest expenditure</t>
   </si>
   <si>
-    <t>cost type</t>
+    <t>Cost type</t>
   </si>
 </sst>
 </file>
@@ -63,7 +63,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,12 +82,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -101,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -111,7 +105,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,13 +385,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -440,18 +439,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
get annual report details
</commit_message>
<xml_diff>
--- a/FinancialPlanningBE/FinancialPlanning.Service/Template/Annual Expense Report.xlsx
+++ b/FinancialPlanningBE/FinancialPlanning.Service/Template/Annual Expense Report.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Year</t>
   </si>
@@ -38,22 +38,29 @@
     <t>Total department</t>
   </si>
   <si>
+    <t>Total Expense</t>
+  </si>
+  <si>
     <t>Department</t>
   </si>
   <si>
-    <t>Total Expense</t>
-  </si>
-  <si>
-    <t>Biggest expenditure</t>
-  </si>
-  <si>
-    <t>Cost type</t>
+    <t>Total expense</t>
+  </si>
+  <si>
+    <t>Biggest expense</t>
+  </si>
+  <si>
+    <t>Cost Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,7 +85,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -95,16 +102,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,61 +397,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="22.26953125" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B5" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>